<commit_message>
Update Experiment 50 repeticiones.xlsx
</commit_message>
<xml_diff>
--- a/Experimento/Experiment 50 repeticiones.xlsx
+++ b/Experimento/Experiment 50 repeticiones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianmorales/Desktop/ProjectX/Experimento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD8F468-194A-2C42-93E4-30AB163A9B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE19AA6-7059-3A4F-BCFF-900E3AC44974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Integrantes" sheetId="9" r:id="rId1"/>
@@ -3670,7 +3670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43282B43-687E-E14B-831B-4A487A019738}">
   <dimension ref="B1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -7713,8 +7713,8 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9374,7 +9374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7CACF5-72B5-3F4E-9E2A-F5791004C35D}">
   <dimension ref="A1:S151"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="91" workbookViewId="0">
+    <sheetView zoomScale="91" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>